<commit_message>
Add missing taxonomy definitions; fix xls typos.
</commit_message>
<xml_diff>
--- a/v2/AIID_Technical_Taxonomies_v2.xlsx
+++ b/v2/AIID_Technical_Taxonomies_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Incident TEMPLATE breakdown" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="576">
   <si>
     <t xml:space="preserve">AI Tasks</t>
   </si>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">The complaint alleges Google’s face grouping tool, which automatically identifies your face in photos and videos uploaded to Photos, violates Illinois’ Biometric Information Privacy Act (BIPA).</t>
   </si>
   <si>
-    <t xml:space="preserve">Face Recognition</t>
+    <t xml:space="preserve">Face Detection</t>
   </si>
   <si>
     <t xml:space="preserve">Google “is in direct violation” of this law, the complaint claims, as it allegedly collects and analyzes a person’s facial structure in connection with its face grouping feature “without providing notice, obtaining informed written consent or publishing data retention policies.”</t>
@@ -694,9 +694,6 @@
   </si>
   <si>
     <t xml:space="preserve">The researchers chose Obama for their latest work because there were hours of high-definition video of him available online in the public domain. The research team had a neural net analyze millions of frames of video to determine how elements of Obama's face moved as he talked, such as his lips and teeth and wrinkles around his mouth and chin.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Face Detection</t>
   </si>
   <si>
     <t xml:space="preserve">In an artificial neural network, components known as artificial neurons are fed data, and work together to solve a problem such as identifying faces or recognizing speech.</t>
@@ -1891,7 +1888,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m&quot;, &quot;d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1927,12 +1924,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2079,7 +2070,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2116,15 +2107,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2136,15 +2123,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2156,11 +2143,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2168,11 +2155,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2284,7 +2271,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -2546,7 +2533,7 @@
       <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="23.22"/>
   </cols>
@@ -2895,7 +2882,7 @@
       <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -3256,7 +3243,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -3375,7 +3362,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="5" t="s">
-        <v>207</v>
+        <v>54</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>3</v>
@@ -3387,18 +3374,18 @@
         <v>3</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="O6" s="5" t="n">
         <v>2</v>
@@ -3407,24 +3394,24 @@
         <v>4</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H7" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>149</v>
       </c>
       <c r="L7" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="O7" s="5" t="n">
         <v>2</v>
@@ -3433,12 +3420,12 @@
         <v>5</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O8" s="5" t="n">
         <v>2</v>
@@ -3447,7 +3434,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3455,7 +3442,7 @@
         <v>137</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O9" s="5" t="n">
         <v>3</v>
@@ -3464,7 +3451,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3475,7 +3462,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3486,7 +3473,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3497,7 +3484,7 @@
         <v>10</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3508,7 +3495,7 @@
         <v>11</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,7 +3506,7 @@
         <v>12</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3530,7 +3517,7 @@
         <v>13</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3541,7 +3528,7 @@
         <v>14</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,7 +3539,7 @@
         <v>15</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,7 +3550,7 @@
         <v>16</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,7 +3655,7 @@
       <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -3750,19 +3737,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,13 +3760,13 @@
         <v>3</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3793,30 +3780,30 @@
         <v>3</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>4</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L6" s="5" t="n">
         <v>2</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P6" s="7" t="n">
         <v>4</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,13 +3820,13 @@
         <v>1</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3847,7 +3834,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3848,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,7 +4001,7 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="22.81"/>
@@ -4100,30 +4087,30 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>246</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="O3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="O3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4134,7 +4121,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O4" s="7" t="n">
         <v>1</v>
@@ -4143,7 +4130,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,7 +4141,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,7 +4152,7 @@
         <v>4</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4163,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,12 +4174,12 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N9" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O9" s="7" t="n">
         <v>1</v>
@@ -4201,7 +4188,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4196,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4217,7 +4204,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4225,16 +4212,16 @@
         <v>183</v>
       </c>
       <c r="L12" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="P12" s="7" t="n">
         <v>10</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4229,7 @@
         <v>11</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4375,7 +4362,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="5" width="32.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="19.88"/>
@@ -4471,21 +4458,21 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="101.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>267</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>10</v>
@@ -4493,47 +4480,47 @@
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="12" t="s">
-        <v>268</v>
+      <c r="Q3" s="11" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>271</v>
+      <c r="Q4" s="12" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P5" s="7" t="n">
         <v>3</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="623.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="13" t="s">
-        <v>275</v>
+      <c r="Q6" s="12" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4541,33 +4528,33 @@
         <v>198</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K8" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L8" s="7" t="n">
         <v>7</v>
       </c>
       <c r="M8" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="N8" s="13" t="s">
         <v>279</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>280</v>
       </c>
       <c r="P8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="13" t="s">
-        <v>281</v>
+      <c r="Q8" s="12" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4575,40 +4562,40 @@
         <v>93</v>
       </c>
       <c r="L9" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="P9" s="7" t="n">
         <v>7</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I10" s="7" t="n">
         <v>8</v>
       </c>
       <c r="K10" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="M10" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>288</v>
       </c>
       <c r="P10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="Q10" s="12" t="s">
-        <v>289</v>
+      <c r="Q10" s="11" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="76.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,8 +4604,8 @@
       <c r="P11" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="13" t="s">
-        <v>290</v>
+      <c r="Q11" s="12" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4632,43 +4619,43 @@
         <v>10</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P13" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="Q13" s="13" t="s">
-        <v>292</v>
+      <c r="Q13" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K14" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="L14" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="M14" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="P14" s="7" t="n">
         <v>12</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="L15" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="M15" s="7" t="s">
         <v>298</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>299</v>
       </c>
       <c r="P15" s="7" t="n">
         <v>13</v>
@@ -4676,7 +4663,7 @@
     </row>
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L16" s="7" t="n">
         <v>2</v>
@@ -4684,8 +4671,8 @@
       <c r="P16" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="Q16" s="13" t="s">
-        <v>301</v>
+      <c r="Q16" s="12" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4699,27 +4686,27 @@
       <c r="P17" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="Q17" s="13" t="s">
-        <v>302</v>
+      <c r="Q17" s="12" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N18" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P18" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="Q18" s="13" t="s">
-        <v>304</v>
+      <c r="Q18" s="12" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="Q19" s="14" t="s">
-        <v>305</v>
+      <c r="Q19" s="13" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4812,7 +4799,7 @@
       <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="5.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="5" width="5.88"/>
@@ -4909,38 +4896,38 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
+      <c r="O3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="O3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="J4" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="11" t="s">
         <v>311</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>312</v>
       </c>
       <c r="O4" s="4" t="n">
         <v>1</v>
@@ -4949,7 +4936,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4957,10 +4944,10 @@
         <v>86</v>
       </c>
       <c r="L5" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>314</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>315</v>
       </c>
       <c r="O5" s="4" t="n">
         <v>2</v>
@@ -4968,8 +4955,8 @@
       <c r="P5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="13" t="s">
-        <v>316</v>
+      <c r="Q5" s="12" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4977,10 +4964,10 @@
         <v>93</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>317</v>
+        <v>310</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>316</v>
       </c>
       <c r="O6" s="4" t="n">
         <v>2</v>
@@ -4988,8 +4975,8 @@
       <c r="P6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="13" t="s">
-        <v>318</v>
+      <c r="Q6" s="12" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4999,13 +4986,13 @@
       <c r="P7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="12" t="s">
-        <v>319</v>
+      <c r="Q7" s="11" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>6</v>
@@ -5017,12 +5004,12 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>6</v>
@@ -5033,8 +5020,8 @@
       <c r="P9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="13" t="s">
-        <v>322</v>
+      <c r="Q9" s="12" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5046,7 +5033,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5054,7 +5041,7 @@
         <v>114</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O11" s="4" t="n">
         <v>8</v>
@@ -5062,8 +5049,8 @@
       <c r="P11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="12" t="s">
-        <v>325</v>
+      <c r="Q11" s="11" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,7 +5061,7 @@
         <v>10</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5084,19 +5071,19 @@
       <c r="P13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Q13" s="13" t="s">
-        <v>327</v>
+      <c r="Q13" s="12" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>329</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>330</v>
       </c>
       <c r="O14" s="4" t="n">
         <v>12</v>
@@ -5105,7 +5092,7 @@
         <v>12</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,10 +5100,10 @@
         <v>198</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="M15" s="7" t="s">
         <v>332</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>333</v>
       </c>
       <c r="O15" s="4" t="n">
         <v>13</v>
@@ -5124,19 +5111,19 @@
       <c r="P15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="Q15" s="13" t="s">
-        <v>334</v>
+      <c r="Q15" s="12" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H16" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="M16" s="7" t="s">
         <v>336</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>337</v>
       </c>
       <c r="O16" s="4" t="n">
         <v>15</v>
@@ -5145,18 +5132,18 @@
         <v>14</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="M17" s="7" t="s">
         <v>339</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>340</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="n">
@@ -5166,10 +5153,10 @@
         <v>15</v>
       </c>
       <c r="Q17" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="R17" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,8 +5166,8 @@
       <c r="P18" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="Q18" s="13" t="s">
-        <v>343</v>
+      <c r="Q18" s="12" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5191,7 +5178,7 @@
         <v>17</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,7 +5189,7 @@
         <v>18</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5213,7 +5200,7 @@
         <v>19</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5224,7 +5211,7 @@
         <v>20</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5235,7 +5222,7 @@
         <v>21</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -5268,7 +5255,7 @@
       <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="5" width="32.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="19.88"/>
@@ -5362,10 +5349,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>349</v>
-      </c>
-      <c r="B3" s="20"/>
+      <c r="A3" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="19"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="n">
@@ -5374,16 +5361,16 @@
       <c r="P3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="13" t="s">
-        <v>350</v>
+      <c r="Q3" s="12" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>351</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>352</v>
       </c>
       <c r="O4" s="4" t="n">
         <v>1</v>
@@ -5392,7 +5379,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5403,13 +5390,13 @@
         <v>3</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O6" s="4" t="n">
         <v>1</v>
@@ -5417,8 +5404,8 @@
       <c r="P6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="13" t="s">
-        <v>356</v>
+      <c r="Q6" s="12" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5429,7 +5416,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5440,7 +5427,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5448,7 +5435,7 @@
         <v>93</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="O9" s="4" t="n">
         <v>1</v>
@@ -5456,8 +5443,8 @@
       <c r="P9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="13" t="s">
-        <v>360</v>
+      <c r="Q9" s="12" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5465,11 +5452,11 @@
         <v>151</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O10" s="4" t="n">
         <v>2</v>
@@ -5478,7 +5465,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5489,7 +5476,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5500,10 +5487,10 @@
         <v>10</v>
       </c>
       <c r="M12" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="O12" s="4" t="n">
         <v>2</v>
@@ -5512,7 +5499,7 @@
         <v>10</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5522,15 +5509,15 @@
       <c r="P13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Q13" s="13" t="s">
-        <v>368</v>
+      <c r="Q13" s="12" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O14" s="4" t="n">
         <v>2</v>
@@ -5538,19 +5525,19 @@
       <c r="P14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="Q14" s="13" t="s">
-        <v>370</v>
+      <c r="Q14" s="12" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K15" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L15" s="4" t="n">
         <v>13</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O15" s="4" t="n">
         <v>2</v>
@@ -5559,13 +5546,13 @@
         <v>13</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M16" s="4"/>
       <c r="N16" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O16" s="4" t="n">
         <v>2</v>
@@ -5574,25 +5561,24 @@
         <v>14</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="E17" s="0"/>
+        <v>375</v>
+      </c>
       <c r="F17" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I17" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="N17" s="21" t="s">
-        <v>378</v>
+      <c r="N17" s="20" t="s">
+        <v>377</v>
       </c>
       <c r="O17" s="4" t="n">
         <v>2</v>
@@ -5601,15 +5587,15 @@
         <v>15</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K18" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4" t="n">
@@ -5619,7 +5605,7 @@
         <v>16</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5630,7 +5616,7 @@
         <v>17</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5641,12 +5627,12 @@
         <v>18</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N21" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O21" s="4" t="n">
         <v>3</v>
@@ -5654,8 +5640,8 @@
       <c r="P21" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="Q21" s="13" t="s">
-        <v>385</v>
+      <c r="Q21" s="12" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5665,8 +5651,8 @@
       <c r="P22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q22" s="13" t="s">
-        <v>386</v>
+      <c r="Q22" s="12" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,10 +5660,10 @@
         <v>185</v>
       </c>
       <c r="L23" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>387</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>388</v>
       </c>
       <c r="O23" s="4" t="n">
         <v>3</v>
@@ -5686,12 +5672,12 @@
         <v>21</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N24" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O24" s="4" t="n">
         <v>3</v>
@@ -5699,13 +5685,13 @@
       <c r="P24" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="Q24" s="13" t="s">
-        <v>391</v>
+      <c r="Q24" s="12" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N25" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O25" s="4" t="n">
         <v>4</v>
@@ -5714,12 +5700,12 @@
         <v>23</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K26" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L26" s="4" t="n">
         <v>24</v>
@@ -5731,7 +5717,7 @@
         <v>24</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5742,7 +5728,7 @@
         <v>25</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5753,7 +5739,7 @@
         <v>26</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5764,7 +5750,7 @@
         <v>27</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5775,7 +5761,7 @@
         <v>28</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5786,7 +5772,7 @@
         <v>29</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5797,12 +5783,12 @@
         <v>30</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N33" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O33" s="4" t="n">
         <v>6</v>
@@ -5811,12 +5797,12 @@
         <v>31</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N34" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="O34" s="4" t="n">
         <v>6</v>
@@ -5824,8 +5810,8 @@
       <c r="P34" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Q34" s="13" t="s">
-        <v>404</v>
+      <c r="Q34" s="12" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +5822,7 @@
         <v>33</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5847,7 +5833,7 @@
         <v>34</v>
       </c>
       <c r="Q36" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5858,7 +5844,7 @@
         <v>35</v>
       </c>
       <c r="Q37" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -5891,7 +5877,7 @@
       <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -5972,28 +5958,28 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>1</v>
@@ -6005,7 +5991,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6016,7 +6002,7 @@
         <v>4</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="O5" s="4" t="n">
         <v>1</v>
@@ -6025,7 +6011,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6035,13 +6021,13 @@
       <c r="P6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="13" t="s">
-        <v>414</v>
+      <c r="Q6" s="12" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H7" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I7" s="5" t="n">
         <v>1</v>
@@ -6053,7 +6039,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6065,7 +6051,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6073,7 +6059,7 @@
         <v>93</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O9" s="4" t="n">
         <v>3</v>
@@ -6082,18 +6068,18 @@
         <v>7</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K10" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="M10" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="O10" s="4" t="n">
         <v>3</v>
@@ -6102,7 +6088,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6113,7 +6099,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -6146,7 +6132,7 @@
       <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="19.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="21.75"/>
@@ -6231,11 +6217,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>424</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>69</v>
@@ -6244,7 +6230,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L3" s="7" t="n">
         <v>1</v>
@@ -6255,8 +6241,8 @@
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="22" t="s">
-        <v>425</v>
+      <c r="Q3" s="21" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6264,10 +6250,10 @@
         <v>89</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>426</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>427</v>
       </c>
       <c r="O4" s="7" t="n">
         <v>1</v>
@@ -6275,13 +6261,13 @@
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="22" t="s">
-        <v>428</v>
+      <c r="Q4" s="21" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>1</v>
@@ -6290,7 +6276,7 @@
         <v>111</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O5" s="7" t="n">
         <v>2</v>
@@ -6299,7 +6285,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6310,12 +6296,12 @@
         <v>4</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G7" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I7" s="7" t="n">
         <v>5</v>
@@ -6327,15 +6313,15 @@
         <v>5</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H8" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>434</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>435</v>
       </c>
       <c r="O8" s="7" t="n">
         <v>2</v>
@@ -6344,7 +6330,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6355,7 +6341,7 @@
         <v>5</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O9" s="7" t="n">
         <v>2</v>
@@ -6364,7 +6350,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6375,7 +6361,7 @@
         <v>6</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O10" s="7" t="n">
         <v>2</v>
@@ -6384,7 +6370,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6395,7 +6381,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6406,7 +6392,7 @@
         <v>10</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6417,18 +6403,18 @@
         <v>11</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K14" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L14" s="7" t="n">
         <v>12</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="O14" s="7" t="n">
         <v>2</v>
@@ -6437,7 +6423,7 @@
         <v>12</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6447,8 +6433,8 @@
       <c r="P15" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="Q15" s="12" t="s">
-        <v>446</v>
+      <c r="Q15" s="11" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6459,7 +6445,7 @@
         <v>14</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6476,7 +6462,7 @@
         <v>15</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6484,7 +6470,7 @@
         <v>16</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6492,7 +6478,7 @@
         <v>17</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6611,11 +6597,11 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -6696,39 +6682,39 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="I3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="0" t="s">
+      <c r="L4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="P4" s="7" t="n">
@@ -6739,19 +6725,19 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="0" t="s">
+      <c r="L5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="P5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6759,7 +6745,7 @@
       <c r="P6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -6767,7 +6753,7 @@
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6775,7 +6761,7 @@
       <c r="P8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -6934,7 +6920,7 @@
       <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="18.51"/>
   </cols>
@@ -7018,26 +7004,26 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>451</v>
+      <c r="A3" s="9" t="s">
+        <v>450</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="L3" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>453</v>
-      </c>
-      <c r="O3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7048,7 +7034,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O4" s="7" t="n">
         <v>1</v>
@@ -7057,7 +7043,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7068,7 +7054,7 @@
         <v>4</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="O5" s="7" t="n">
         <v>2</v>
@@ -7077,12 +7063,12 @@
         <v>3</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O6" s="7" t="n">
         <v>3</v>
@@ -7091,12 +7077,12 @@
         <v>4</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="O7" s="7" t="n">
         <v>3</v>
@@ -7105,18 +7091,18 @@
         <v>5</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K8" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L8" s="7" t="n">
         <v>6</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O8" s="7" t="n">
         <v>3</v>
@@ -7125,18 +7111,18 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K9" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L9" s="7" t="n">
         <v>6</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O9" s="7" t="n">
         <v>3</v>
@@ -7145,7 +7131,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7156,7 +7142,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7289,7 +7275,7 @@
       <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="30.5"/>
   </cols>
@@ -7373,29 +7359,29 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>467</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>468</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>198</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="O3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>468</v>
-      </c>
-      <c r="O3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7405,8 +7391,8 @@
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="12" t="s">
-        <v>470</v>
+      <c r="Q4" s="11" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7417,7 +7403,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7428,7 +7414,7 @@
         <v>4</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7439,7 +7425,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7450,7 +7436,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7458,13 +7444,13 @@
         <v>114</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>86</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O9" s="5" t="n">
         <v>1</v>
@@ -7473,7 +7459,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7629,7 +7615,7 @@
       <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -7710,14 +7696,14 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>477</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>478</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>1</v>
@@ -7735,7 +7721,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7752,12 +7738,12 @@
         <v>2</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>1</v>
@@ -7769,7 +7755,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7780,7 +7766,7 @@
         <v>4</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7791,7 +7777,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7802,7 +7788,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7810,7 +7796,7 @@
         <v>23</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O9" s="5" t="n">
         <v>1</v>
@@ -7819,7 +7805,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7830,7 +7816,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7838,7 +7824,7 @@
         <v>130</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O11" s="5" t="n">
         <v>1</v>
@@ -7847,7 +7833,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7858,7 +7844,7 @@
         <v>10</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7869,7 +7855,7 @@
         <v>11</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8002,7 +7988,7 @@
       <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="24.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="5" width="26.39"/>
@@ -8087,13 +8073,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>492</v>
+      <c r="A3" s="9" t="s">
+        <v>491</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>1</v>
@@ -8105,7 +8091,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="78.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8120,8 +8106,8 @@
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="12" t="s">
-        <v>494</v>
+      <c r="Q4" s="11" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8130,7 +8116,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7" t="n">
@@ -8140,7 +8126,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8154,10 +8140,10 @@
         <v>9</v>
       </c>
       <c r="M6" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>497</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>498</v>
       </c>
       <c r="O6" s="7" t="n">
         <v>1</v>
@@ -8166,7 +8152,7 @@
         <v>4</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8183,15 +8169,15 @@
         <v>5</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H8" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O8" s="7" t="n">
         <v>2</v>
@@ -8200,7 +8186,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8208,7 +8194,7 @@
         <v>198</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O9" s="7" t="n">
         <v>2</v>
@@ -8217,7 +8203,7 @@
         <v>7</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8234,7 +8220,7 @@
         <v>8</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8245,7 +8231,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8388,7 +8374,7 @@
       <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="26.25"/>
@@ -8397,41 +8383,41 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>506</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>507</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>508</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
@@ -8445,7 +8431,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D4" s="0"/>
     </row>
@@ -8455,7 +8441,7 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -8464,13 +8450,13 @@
         <v>151</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>513</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8479,103 +8465,103 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>516</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>517</v>
       </c>
       <c r="D8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>521</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>524</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>526</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8584,22 +8570,22 @@
         <v>130</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>530</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8608,10 +8594,10 @@
         <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>532</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8619,16 +8605,16 @@
         <v>86</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D20" s="0"/>
     </row>
@@ -8637,7 +8623,7 @@
         <v>183</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D21" s="0"/>
     </row>
@@ -8663,102 +8649,102 @@
       <c r="D28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
-        <v>537</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="27"/>
-      <c r="AA29" s="27"/>
+      <c r="A29" s="25" t="s">
+        <v>536</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>539</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>540</v>
       </c>
       <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>543</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>544</v>
       </c>
       <c r="D34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D36" s="7"/>
     </row>
@@ -8767,42 +8753,42 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C38" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>547</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>198</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D41" s="0"/>
     </row>
@@ -8811,77 +8797,77 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>552</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>553</v>
       </c>
       <c r="D43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="23" t="s">
         <v>556</v>
       </c>
-      <c r="D45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="24" t="s">
-        <v>557</v>
-      </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="25"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25"/>
-      <c r="T46" s="25"/>
-      <c r="U46" s="25"/>
-      <c r="V46" s="25"/>
-      <c r="W46" s="25"/>
-      <c r="X46" s="25"/>
-      <c r="Y46" s="25"/>
-      <c r="Z46" s="25"/>
-      <c r="AA46" s="25"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="24"/>
+      <c r="Z46" s="24"/>
+      <c r="AA46" s="24"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>558</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8892,7 +8878,7 @@
         <v>84</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D49" s="0"/>
     </row>
@@ -8902,31 +8888,31 @@
         <v>134</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D52" s="0"/>
     </row>
@@ -8935,63 +8921,63 @@
         <v>114</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>565</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D59" s="0"/>
     </row>
@@ -9003,10 +8989,10 @@
         <v>175</v>
       </c>
       <c r="C61" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>572</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9017,13 +9003,13 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D65" s="0"/>
     </row>
@@ -9032,7 +9018,7 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -9062,7 +9048,7 @@
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -9143,146 +9129,146 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="I3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="0" t="n">
+      <c r="I4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="5" t="n">
         <v>3</v>
       </c>
       <c r="P5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="5" t="n">
         <v>3</v>
       </c>
       <c r="P6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="5" t="n">
         <v>3</v>
       </c>
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="5" t="n">
         <v>3</v>
       </c>
       <c r="P8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="0" t="s">
+      <c r="L9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="5" t="n">
         <v>3</v>
       </c>
       <c r="P9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K10" s="0" t="s">
+      <c r="K10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="0" t="s">
+      <c r="L10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" s="5" t="s">
         <v>46</v>
       </c>
       <c r="P10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N11" s="0" t="s">
+      <c r="N11" s="5" t="s">
         <v>48</v>
       </c>
       <c r="P11" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -9423,10 +9409,10 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -9507,50 +9493,50 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="I3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P5" s="7" t="n">
@@ -9727,9 +9713,9 @@
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="51.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="5" width="51.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9811,164 +9797,164 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N5" s="0" t="s">
+      <c r="N5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="5" t="n">
         <v>4</v>
       </c>
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="5" t="n">
         <v>4</v>
       </c>
       <c r="P8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="5" t="n">
         <v>4</v>
       </c>
       <c r="P9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="5" t="n">
         <v>5</v>
       </c>
       <c r="P10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="M11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="5" t="n">
         <v>5</v>
       </c>
       <c r="P11" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="5" t="n">
         <v>7</v>
       </c>
       <c r="P12" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="0" t="s">
+      <c r="K13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="0" t="s">
+      <c r="L13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="5" t="n">
         <v>7</v>
       </c>
       <c r="P13" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O14" s="0" t="n">
+      <c r="O14" s="5" t="n">
         <v>8</v>
       </c>
       <c r="P14" s="7" t="n">
@@ -9979,35 +9965,35 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O15" s="0" t="n">
+      <c r="O15" s="5" t="n">
         <v>8</v>
       </c>
       <c r="P15" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="5" t="n">
         <v>8</v>
       </c>
       <c r="P16" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O17" s="0" t="n">
+      <c r="O17" s="5" t="n">
         <v>22</v>
       </c>
       <c r="P17" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -10121,7 +10107,7 @@
       <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -10202,76 +10188,76 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="L5" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P6" s="7" t="n">
@@ -10282,79 +10268,79 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P11" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P12" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P13" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" s="5" t="s">
         <v>103</v>
       </c>
     </row>
@@ -10484,11 +10470,11 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -10569,16 +10555,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="7" t="n">
@@ -10589,136 +10575,136 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="L7" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="P9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="5" t="n">
         <v>4</v>
       </c>
       <c r="P10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="5" t="n">
         <v>4</v>
       </c>
       <c r="P11" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="5" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="5" t="n">
         <v>4</v>
       </c>
       <c r="P12" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="0" t="s">
+      <c r="L13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="5" t="n">
         <v>6</v>
       </c>
       <c r="P13" s="7" t="n">
@@ -10729,89 +10715,89 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="L14" s="0" t="s">
+      <c r="L14" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="O14" s="5" t="n">
         <v>9</v>
       </c>
       <c r="P14" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="0" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="L15" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="O15" s="5" t="n">
         <v>9</v>
       </c>
       <c r="P15" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="5" t="n">
         <v>10</v>
       </c>
       <c r="P16" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O17" s="0" t="n">
+      <c r="O17" s="5" t="n">
         <v>10</v>
       </c>
       <c r="P17" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="O18" s="0" t="n">
+      <c r="O18" s="5" t="n">
         <v>11</v>
       </c>
       <c r="P18" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L19" s="0" t="n">
+      <c r="L19" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="O19" s="5" t="n">
         <v>11</v>
       </c>
       <c r="P19" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="Q19" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -10915,7 +10901,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
@@ -11348,7 +11334,7 @@
       <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">

</xml_diff>